<commit_message>
Display test method name in extent report
</commit_message>
<xml_diff>
--- a/EcommerceDemoTestcases.xlsx
+++ b/EcommerceDemoTestcases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonn\Desktop\training courses\EcommerceDemo_Selenium_CSharp_Automation_Framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonn\Desktop\projects\EcommerceDemo_Selenium_CSharp_Automation_Framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9638375E-17F5-4D48-993F-70A4997A8C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02776703-B585-4A8E-BA59-9CF6EE8F31F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="83">
   <si>
     <t>Project Name:</t>
   </si>
@@ -591,9 +591,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -638,6 +635,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1054,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1156,55 +1156,55 @@
       <c r="A6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
       <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="7"/>
@@ -1216,339 +1216,363 @@
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="K10" s="16" t="s">
+      <c r="K10" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="78" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="19"/>
-      <c r="H11" s="18" t="s">
+      <c r="G11" s="18"/>
+      <c r="H11" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="J11" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="21"/>
+      <c r="K11" s="20"/>
     </row>
     <row r="12" spans="1:11" ht="78" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="J12" s="22" t="s">
+      <c r="J12" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="K12" s="25"/>
+      <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:11" ht="78" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="G13" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H13" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="I13" s="24" t="s">
+      <c r="I13" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="J13" s="22" t="s">
+      <c r="J13" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="K13" s="25"/>
+      <c r="K13" s="24"/>
     </row>
     <row r="14" spans="1:11" ht="78" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24" t="s">
+      <c r="G14" s="23"/>
+      <c r="H14" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="24" t="s">
+      <c r="I14" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="J14" s="22" t="s">
+      <c r="J14" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="K14" s="25"/>
+      <c r="K14" s="24"/>
     </row>
     <row r="15" spans="1:11" ht="78" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="22"/>
-      <c r="H15" s="26" t="s">
+      <c r="G15" s="21"/>
+      <c r="H15" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="25"/>
+      <c r="I15" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="24"/>
     </row>
     <row r="16" spans="1:11" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="25"/>
+      <c r="I16" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" s="24"/>
     </row>
     <row r="17" spans="1:11" ht="156" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="G17" s="24" t="s">
+      <c r="G17" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="H17" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="27" t="s">
+      <c r="I17" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="J17" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" s="26" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="G18" s="22"/>
-      <c r="H18" s="18" t="s">
+      <c r="G18" s="21"/>
+      <c r="H18" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="25"/>
+      <c r="I18" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" s="24"/>
     </row>
     <row r="19" spans="1:11" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="G19" s="24" t="s">
+      <c r="G19" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="25"/>
-    </row>
-    <row r="20" spans="1:11" ht="156" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
+      <c r="I19" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="J19" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19" s="24"/>
+    </row>
+    <row r="20" spans="1:11" ht="171.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="G20" s="24" t="s">
+      <c r="G20" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="H20" s="24" t="s">
+      <c r="H20" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="25"/>
+      <c r="I20" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="24"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
@@ -1563,7 +1587,7 @@
       <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="28"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="7"/>
@@ -1575,7 +1599,7 @@
       <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="28"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="7"/>

</xml_diff>